<commit_message>
Terminando primera pasada de la presentacion =)
</commit_message>
<xml_diff>
--- a/Tesis/Imagenes/Fuentes/04/XeY.xlsx
+++ b/Tesis/Imagenes/Fuentes/04/XeY.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Neo Zero\UBA\Dropbox\Tesis\Actual\Documento\Tesis\Imagenes\Fuentes\04\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Tesis\ActualGit\Tesis\Imagenes\Fuentes\04\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9580" windowHeight="3060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9585" windowHeight="3060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Grafico" sheetId="2" r:id="rId1"/>
+    <sheet name="Grafico (2)" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>Trials\Features</t>
   </si>
@@ -72,6 +73,21 @@
   </si>
   <si>
     <t>r3</t>
+  </si>
+  <si>
+    <t>Muestras\Features</t>
+  </si>
+  <si>
+    <t>Muestra 1</t>
+  </si>
+  <si>
+    <t>Muestra 2</t>
+  </si>
+  <si>
+    <t>Muestra 3</t>
+  </si>
+  <si>
+    <t>Muestra n</t>
   </si>
 </sst>
 </file>
@@ -395,6 +411,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -402,14 +426,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -704,8 +720,283 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>149412</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>59764</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>291353</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>141941</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Right Arrow 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4359462" y="850339"/>
+          <a:ext cx="141941" cy="82177"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-AR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152404</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>55284</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>294345</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>137461</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Right Arrow 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4362454" y="1036359"/>
+          <a:ext cx="141941" cy="82177"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-AR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>147918</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>50803</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>289859</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>132980</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Right Arrow 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4357968" y="1222378"/>
+          <a:ext cx="141941" cy="82177"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-AR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>158370</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>46321</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>300311</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>128498</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Right Arrow 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4368420" y="1408396"/>
+          <a:ext cx="141941" cy="82177"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-AR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>153884</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>34371</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>295825</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>116548</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Right Arrow 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4363934" y="1586946"/>
+          <a:ext cx="141941" cy="82177"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-AR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -969,43 +1260,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.08984375" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" customWidth="1"/>
-    <col min="7" max="7" width="6.6328125" customWidth="1"/>
-    <col min="8" max="8" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="12" t="s">
+    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="16" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="17"/>
-    </row>
-    <row r="4" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="14"/>
+    </row>
+    <row r="4" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1021,12 +1312,12 @@
       <c r="F4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="15"/>
+      <c r="G4" s="12"/>
       <c r="H4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
@@ -1034,12 +1325,12 @@
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
-      <c r="G5" s="15"/>
+      <c r="G5" s="12"/>
       <c r="H5" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
@@ -1047,12 +1338,12 @@
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
-      <c r="G6" s="15"/>
+      <c r="G6" s="12"/>
       <c r="H6" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
@@ -1060,12 +1351,12 @@
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
-      <c r="G7" s="15"/>
+      <c r="G7" s="12"/>
       <c r="H7" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
@@ -1073,12 +1364,12 @@
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
-      <c r="G8" s="15"/>
+      <c r="G8" s="12"/>
       <c r="H8" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>9</v>
       </c>
@@ -1086,65 +1377,246 @@
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
-      <c r="G9" s="15"/>
+      <c r="G9" s="12"/>
       <c r="H9" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="5.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="I13" s="18"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="I14" s="15"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="I15" s="15"/>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="I16" s="15"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="I17" s="15"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="I18" s="15"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="I19" s="15"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="I20" s="15"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
+    <row r="10" spans="2:9" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I13" s="15"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I14" s="12"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I15" s="12"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I16" s="12"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I18" s="12"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I19" s="12"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I20" s="12"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:I23"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="14"/>
+    </row>
+    <row r="4" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="2:9" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I13" s="15"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I14" s="12"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I15" s="12"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I16" s="12"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I18" s="12"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I19" s="12"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I20" s="12"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>